<commit_message>
library records stats edits
</commit_message>
<xml_diff>
--- a/library-records-dataset/data-statistics/distinct_subject_domains.xlsx
+++ b/library-records-dataset/data-statistics/distinct_subject_domains.xlsx
@@ -1,45 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSouzaJ\Datasets\subject-indexing-dataset\library-records-dataset\data-statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SadruddinS\Data\GermEval25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC5FBA1-70C2-436F-87C6-253304D7DF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="2820" windowWidth="19464" windowHeight="9912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -47,9 +32,6 @@
     <t>IRI</t>
   </si>
   <si>
-    <t>Full Form</t>
-  </si>
-  <si>
     <t>https://purl.org/linsearch/ver</t>
   </si>
   <si>
@@ -222,13 +204,106 @@
   </si>
   <si>
     <t>Sports Science</t>
+  </si>
+  <si>
+    <t>Full Form (English)</t>
+  </si>
+  <si>
+    <t>Full Form (German)</t>
+  </si>
+  <si>
+    <t>Architektur</t>
+  </si>
+  <si>
+    <t>Bauwesen</t>
+  </si>
+  <si>
+    <t>Bergbau</t>
+  </si>
+  <si>
+    <t>Biowissenschaften, Biologie</t>
+  </si>
+  <si>
+    <t>Chemische und Umwelttechnik</t>
+  </si>
+  <si>
+    <t>Chemie</t>
+  </si>
+  <si>
+    <t>Elektrotechnik</t>
+  </si>
+  <si>
+    <t>Werkstoffkunde</t>
+  </si>
+  <si>
+    <t>Geowissenschaften, Geographie</t>
+  </si>
+  <si>
+    <t>Geschichte</t>
+  </si>
+  <si>
+    <t>Gartenbau</t>
+  </si>
+  <si>
+    <t>Informatik</t>
+  </si>
+  <si>
+    <t>Rechtswissenschaften</t>
+  </si>
+  <si>
+    <t>Sprachwissenschaften</t>
+  </si>
+  <si>
+    <t>Literaturwissenschaften</t>
+  </si>
+  <si>
+    <t>Maschinenbau, Energietechnik</t>
+  </si>
+  <si>
+    <t>Mathematik</t>
+  </si>
+  <si>
+    <t>Medizintechnik</t>
+  </si>
+  <si>
+    <t>Medizin</t>
+  </si>
+  <si>
+    <t>Wirtschaftswissenschaften</t>
+  </si>
+  <si>
+    <t>Erziehungswissenschaften, Fachdidaktiken</t>
+  </si>
+  <si>
+    <t>Philosophie</t>
+  </si>
+  <si>
+    <t>Physik</t>
+  </si>
+  <si>
+    <t>Religionswissenschaft, Theologie</t>
+  </si>
+  <si>
+    <t>Konnte nicht zugeordnet werden</t>
+  </si>
+  <si>
+    <t>Sozialwissenschaften</t>
+  </si>
+  <si>
+    <t>Sportwissenschaft</t>
+  </si>
+  <si>
+    <t>Technik allgemein</t>
+  </si>
+  <si>
+    <t>Verkehrstechnik, Verkehrswesen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,14 +315,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,19 +337,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,11 +624,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,9 +636,10 @@
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,349 +647,436 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>RIGHT(B2, 3)</f>
         <v>arc</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A30" si="0">RIGHT(B3, 3)</f>
+        <v>bau</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A29" si="0">RIGHT(B3, 3)</f>
-        <v>bau</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>che</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>che</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>elt</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>elt</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>fer</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>fer</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>his</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f t="shared" si="0"/>
-        <v>his</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>inf</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>inf</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>lin</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>lin</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>lit</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>lit</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>mat</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>mat</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>oek</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>oek</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>pae</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>pae</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>phi</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>phi</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>phy</v>
+      </c>
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>phy</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>sow</v>
+      </c>
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>sow</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>tec</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v>tec</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>ver</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>ber</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <f t="shared" si="0"/>
-        <v>ver</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f t="shared" si="0"/>
-        <v>ber</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>bio</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>bio</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>cet</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>cet</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>geo</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>geo</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>hor</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>hor</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>jur</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>jur</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>mas</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>mas</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>med</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>med</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>RIGHT(B27, 4)</f>
         <v>meda</v>
       </c>
       <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>rel</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>rel</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>RIGHT(B29, 4)</f>
+        <v>rest</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>spo</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f>RIGHT(B30, 4)</f>
-        <v>rest</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
@@ -932,12 +1084,12 @@
       <c r="C30" t="s">
         <v>59</v>
       </c>
+      <c r="D30" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FDD43660-EDDD-4DD5-B1D7-998747C4D0B5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>